<commit_message>
Change collapsed button and add is active in item price import
</commit_message>
<xml_diff>
--- a/client/src/assets/sample/ctordering_items_price.xlsx
+++ b/client/src/assets/sample/ctordering_items_price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sc01/ruby/order-system/client/src/assets/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ED6220-D349-E34C-A57B-5C0C4D36C6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA945EE6-8F8C-4646-9AD2-7CC4B5B5C7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Price</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>ItemCode</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -410,16 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -429,6 +434,9 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>